<commit_message>
Revert "dist displays rewrite"
This reverts commit a7e4e721b98d0f9fff4c47b2e127d1c803d74bb9.
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/KPI Overview Molson Coors v5.3.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/KPI Overview Molson Coors v5.3.xlsx
@@ -4239,7 +4239,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="bottomRight" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4462,10 +4462,10 @@
         <v>76</v>
       </c>
       <c r="J3" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="42" t="s">
         <v>92</v>
-      </c>
-      <c r="K3" s="51" t="s">
-        <v>76</v>
       </c>
       <c r="L3" s="43" t="s">
         <v>76</v>

</xml_diff>